<commit_message>
Fix parsing 'namespace' keyword
</commit_message>
<xml_diff>
--- a/test/Spreadsheet.xlsx
+++ b/test/Spreadsheet.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/works/exclbr/build/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mac/Documents/works/exclbr/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB46653-082F-A944-B685-4C0D80847145}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{766DE8A5-4E85-DE41-BB3B-B872A2282FCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="27320" windowHeight="14860" xr2:uid="{FF49B81A-127A-B44C-A44B-FF0F3EF8FCF9}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>path</t>
   </si>
@@ -46,19 +46,34 @@
   </si>
   <si>
     <t>on_load</t>
+  </si>
+  <si>
+    <t>./file2.cpp(8)</t>
+  </si>
+  <si>
+    <t>osx_source</t>
+  </si>
+  <si>
+    <t>check_error</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,8 +96,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -400,7 +416,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -441,14 +457,26 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="17" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>7</v>
+      </c>
       <c r="C4">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
       <c r="C5">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>